<commit_message>
Update parsing logic to account for cyriclic characters
</commit_message>
<xml_diff>
--- a/mastersheet.xlsx
+++ b/mastersheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I3"/>
+  <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,316 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus extensor digitorum: А. Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>D. Tuberositas radii E. Fascia antebrachii</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Mușchiul extensor al degetelor își are originea pe epicondilul lateral al humerusului și pe fascia antebrațului. Distal mușchiul formează patru tendoane, care se inseră pe fața dorsală a falangelor într-un mod cu totul deosebit.Enunțuri corecte sunt „A” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: А. Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Flexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: А. Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Flexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeriА. Epicondylus lateralis humeriFlexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeriА. Epicondylus lateralis humeriFlexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeriА. Epicondylus lateralis humeriFlexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeriB. Epicondylus medialis humeriC. OlecranonD. Tuberositas radii E. Fascia antebraţuluiА. Epicondylus lateralis humeriB. Epicondylus medialis humeriC. OlecranonD. Tuberositas radii E. Antebrachial fasciaA. Epicondylus lateralis humeriB. Epicondylus medialis humeriC. OlecranonD. Tuberositas radiiE. Фасция предплечьяFlexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Flexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>А. Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>B. Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>C. Olecranon</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">D. Tuberositas radii </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>E. Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Flexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus flexor carpi radialis: </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Olecranon</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Tuberositas radii</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Fascia antebraţului</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Flexorul radial al carpului își ia originea de pe epicondilul medial al humerusului, fascia antebrațului, și de la septele fibroase, care îl separă de pronatorul rotund și palmarul lung și se inseră pe baza osului metacarpian II trecând în prealabil prin canalul radial al carpului de sub retinaculul flexorilor; tendonul lui delimitează șanțul pulsului.Corect – „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Skip appending everything in explanation
</commit_message>
<xml_diff>
--- a/mastersheet.xlsx
+++ b/mastersheet.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -805,6 +805,134 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Originea musculus extensor digitorum: </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Epicondylus lateralis humeri</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Epicondylus medialis humeri</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Olecranon</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Tuberositas radii</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Fascia antebrachii</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Mușchiul extensor al degetelor își are originea pe epicondilul lateral al humerusului și pe fascia antebrațului. Distal mușchiul formează patru tendoane, care se inseră pe fața dorsală a falangelor într-un mod cu totul deosebit.Enunțuri corecte sunt „A” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Muşchii mâinii, eminenţa tenară:</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Se disting muşchii palmari, dorsali şi interosoşi.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sunt situaţi în trei planuri.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Toţi, cu excepţia adductorului policelului, au originea pe rândul proximal al oaselor carpiene.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>M.opozant al policelului se inseră pe primul os metacarpian.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>С. Самой глубокой является м-ца противопостаиляющая большой палец.проксимального ряда.Mușchii mâinii sunt amplasați numai pe fața palmară și în spațiile intermetacarpiene; pe fața dorsală a mâinii se află numai tendoanele mușchilor posteriori ai antebrațului.Mușchii mâinii formează trei grupuri:- lateral (eminența tenară);- medial (eminența hipotenară);- mediu (lombricalii, interosoșii palmari și dorsali).Mușchii eminenței tenare sunt dispuși în trei planuri. În primul plan se află abductorul scurt al policelui, în planul al doilea – apozantul policelui și flexorul scurt al policelui, în planul al treilea – adductorul policelui. Ei au originea unii pe oasele carpiene din rândul I, alții pe carpienele din rândul II, pe metacarpiene și pe retinaculul flexorilor și inserția sau pe osul metacarpian I (mușchiul apozant al policelui), sau pe falanga proximală a policelui. Astfel corecte sunt numai enunțurile „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Muşchii mâinii, eminenţa tenară:</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Se disting muşchii palmari, dorsali şi interosoşi.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sunt situaţi în trei planuri.</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Toţi, cu excepţia adductorului policelului, au originea pe rândul proximal al oaselor carpiene.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>M.opozant al policelului se inseră pe primul os metacarpian.</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Muşchii mâinii, eminenţa tenară:</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Se disting muşchii palmari, dorsali şi interosoşi.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sunt situaţi în trei planuri.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Toţi, cu excepţia adductorului policelului, au originea pe rândul proximal al oaselor carpiene.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>M.opozant al policelului se inseră pe primul os metacarpian.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Mușchii mâinii sunt amplasați numai pe fața palmară și în spațiile intermetacarpiene; pe fața dorsală a mâinii se află numai tendoanele mușchilor posteriori ai antebrațului.Mușchii mâinii formează trei grupuri:- lateral (eminența tenară);- medial (eminența hipotenară);- mediu (lombricalii, interosoșii palmari și dorsali).Mușchii eminenței tenare sunt dispuși în trei planuri. În primul plan se află abductorul scurt al policelui, în planul al doilea – apozantul policelui și flexorul scurt al policelui, în planul al treilea – adductorul policelui. Ei au originea unii pe oasele carpiene din rândul I, alții pe carpienele din rândul II, pe metacarpiene și pe retinaculul flexorilor și inserția sau pe osul metacarpian I (mușchiul apozant al policelui), sau pe falanga proximală a policelui. Astfel corecte sunt numai enunțurile „B” și „E”.</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>